<commit_message>
13th Day - Covariance matrix and Correlation matrix done Before fusion of covid19_graph and clustering_country
</commit_message>
<xml_diff>
--- a/team9/files/dataset_final.xlsx
+++ b/team9/files/dataset_final.xlsx
@@ -380,22 +380,22 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Confirmed.Cases</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Deaths</t>
+          <t>Deaths.Cases</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Press.Liberty</t>
+          <t>Press.Liberty.Index</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>DEMOCRACY.INDEX</t>
+          <t>Democracy.Index</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -434,10 +434,10 @@
         <v>37172386</v>
       </c>
       <c r="E2">
-        <v>3392</v>
+        <v>4033</v>
       </c>
       <c r="F2">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="G2">
         <v>60.54</v>
@@ -446,13 +446,13 @@
         <v>2.55</v>
       </c>
       <c r="I2">
-        <v>2.797775746759974</v>
+        <v>3.093694335359586</v>
       </c>
       <c r="J2">
-        <v>91.25053204817145</v>
+        <v>108.4945152565671</v>
       </c>
       <c r="K2">
-        <v>3.066037735849056</v>
+        <v>2.851475328539549</v>
       </c>
     </row>
     <row r="3">
@@ -475,7 +475,7 @@
         <v>30809762</v>
       </c>
       <c r="E3">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -490,10 +490,10 @@
         <v>0.06491449041378508</v>
       </c>
       <c r="J3">
-        <v>1.168460827448131</v>
+        <v>1.395661543896379</v>
       </c>
       <c r="K3">
-        <v>5.555555555555555</v>
+        <v>4.651162790697675</v>
       </c>
     </row>
     <row r="4">
@@ -516,7 +516,7 @@
         <v>2866376</v>
       </c>
       <c r="E4">
-        <v>832</v>
+        <v>856</v>
       </c>
       <c r="F4">
         <v>31</v>
@@ -531,10 +531,10 @@
         <v>10.81505008414807</v>
       </c>
       <c r="J4">
-        <v>290.2619893551998</v>
+        <v>298.6349313558305</v>
       </c>
       <c r="K4">
-        <v>3.725961538461538</v>
+        <v>3.621495327102803</v>
       </c>
     </row>
     <row r="5">
@@ -557,10 +557,10 @@
         <v>9630959</v>
       </c>
       <c r="E5">
-        <v>15738</v>
+        <v>17417</v>
       </c>
       <c r="F5">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="G5">
         <v>60.61</v>
@@ -569,13 +569,13 @@
         <v>2.69</v>
       </c>
       <c r="I5">
-        <v>16.30159571855721</v>
+        <v>19.20888667473302</v>
       </c>
       <c r="J5">
-        <v>1634.105181010531</v>
+        <v>1808.438806561216</v>
       </c>
       <c r="K5">
-        <v>0.9975854619392553</v>
+        <v>1.06218062812195</v>
       </c>
     </row>
     <row r="6">
@@ -598,10 +598,10 @@
         <v>44494502</v>
       </c>
       <c r="E6">
-        <v>5195</v>
+        <v>5763</v>
       </c>
       <c r="F6">
-        <v>273</v>
+        <v>300</v>
       </c>
       <c r="G6">
         <v>74.93000000000001</v>
@@ -610,13 +610,13 @@
         <v>6.96</v>
       </c>
       <c r="I6">
-        <v>6.135589516205845</v>
+        <v>6.742406061764664</v>
       </c>
       <c r="J6">
-        <v>116.7559983028914</v>
+        <v>129.5216204464992</v>
       </c>
       <c r="K6">
-        <v>5.255052935514918</v>
+        <v>5.205622071837585</v>
       </c>
     </row>
     <row r="7">
@@ -639,10 +639,10 @@
         <v>2951776</v>
       </c>
       <c r="E7">
-        <v>2782</v>
+        <v>3175</v>
       </c>
       <c r="F7">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G7">
         <v>69.62</v>
@@ -651,13 +651,13 @@
         <v>4.11</v>
       </c>
       <c r="I7">
-        <v>13.55116377394491</v>
+        <v>14.9062801513394</v>
       </c>
       <c r="J7">
-        <v>942.4834404778682</v>
+        <v>1075.623624556877</v>
       </c>
       <c r="K7">
-        <v>1.437814521926671</v>
+        <v>1.385826771653543</v>
       </c>
     </row>
     <row r="8">
@@ -680,7 +680,7 @@
         <v>24992369</v>
       </c>
       <c r="E8">
-        <v>6875</v>
+        <v>6929</v>
       </c>
       <c r="F8">
         <v>97</v>
@@ -695,10 +695,10 @@
         <v>3.881184692815635</v>
       </c>
       <c r="J8">
-        <v>275.0839666299741</v>
+        <v>277.2446261496859</v>
       </c>
       <c r="K8">
-        <v>1.410909090909091</v>
+        <v>1.399913407418098</v>
       </c>
     </row>
     <row r="9">
@@ -721,10 +721,10 @@
         <v>8847037</v>
       </c>
       <c r="E9">
-        <v>15651</v>
+        <v>15777</v>
       </c>
       <c r="F9">
-        <v>608</v>
+        <v>615</v>
       </c>
       <c r="G9">
         <v>86.53</v>
@@ -733,13 +733,13 @@
         <v>8.42</v>
       </c>
       <c r="I9">
-        <v>68.72357377956033</v>
+        <v>69.514799135575</v>
       </c>
       <c r="J9">
-        <v>1769.066863855096</v>
+        <v>1783.308920263361</v>
       </c>
       <c r="K9">
-        <v>3.884735799629417</v>
+        <v>3.898079482791405</v>
       </c>
     </row>
     <row r="10">
@@ -762,10 +762,10 @@
         <v>9942334</v>
       </c>
       <c r="E10">
-        <v>2127</v>
+        <v>2422</v>
       </c>
       <c r="F10">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G10">
         <v>43.6</v>
@@ -774,13 +774,13 @@
         <v>2.65</v>
       </c>
       <c r="I10">
-        <v>2.816240130335593</v>
+        <v>3.117980144300121</v>
       </c>
       <c r="J10">
-        <v>213.9336699008502</v>
+        <v>243.6047712740288</v>
       </c>
       <c r="K10">
-        <v>1.316408086506817</v>
+        <v>1.279933938893477</v>
       </c>
     </row>
     <row r="11">
@@ -844,10 +844,10 @@
         <v>11422068</v>
       </c>
       <c r="E12">
-        <v>50781</v>
+        <v>52596</v>
       </c>
       <c r="F12">
-        <v>8339</v>
+        <v>8581</v>
       </c>
       <c r="G12">
         <v>87.25</v>
@@ -856,13 +856,13 @@
         <v>7.78</v>
       </c>
       <c r="I12">
-        <v>730.0779508579357</v>
+        <v>751.2650073524338</v>
       </c>
       <c r="J12">
-        <v>4445.867420855838</v>
+        <v>4604.770344564574</v>
       </c>
       <c r="K12">
-        <v>16.42149622890451</v>
+        <v>16.31492889193095</v>
       </c>
     </row>
     <row r="13">
@@ -885,7 +885,7 @@
         <v>11485048</v>
       </c>
       <c r="E13">
-        <v>102</v>
+        <v>284</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -900,10 +900,10 @@
         <v>0.1741394550549549</v>
       </c>
       <c r="J13">
-        <v>8.881112207802701</v>
+        <v>24.7278026178036</v>
       </c>
       <c r="K13">
-        <v>1.96078431372549</v>
+        <v>0.7042253521126761</v>
       </c>
     </row>
     <row r="14">
@@ -926,7 +926,7 @@
         <v>19751535</v>
       </c>
       <c r="E14">
-        <v>729</v>
+        <v>748</v>
       </c>
       <c r="F14">
         <v>48</v>
@@ -941,10 +941,10 @@
         <v>2.430190868709698</v>
       </c>
       <c r="J14">
-        <v>36.90852381852854</v>
+        <v>37.87047437072613</v>
       </c>
       <c r="K14">
-        <v>6.584362139917696</v>
+        <v>6.417112299465241</v>
       </c>
     </row>
     <row r="15">
@@ -967,10 +967,10 @@
         <v>161356039</v>
       </c>
       <c r="E15">
-        <v>11719</v>
+        <v>13770</v>
       </c>
       <c r="F15">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="G15">
         <v>51.64</v>
@@ -979,13 +979,13 @@
         <v>5.43</v>
       </c>
       <c r="I15">
-        <v>1.152730329479642</v>
+        <v>1.326259626390556</v>
       </c>
       <c r="J15">
-        <v>72.62820823210713</v>
+        <v>85.33922923083158</v>
       </c>
       <c r="K15">
-        <v>1.58716614045567</v>
+        <v>1.554103122730574</v>
       </c>
     </row>
     <row r="16">
@@ -1008,10 +1008,10 @@
         <v>7024216</v>
       </c>
       <c r="E16">
-        <v>1778</v>
+        <v>1955</v>
       </c>
       <c r="F16">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G16">
         <v>64.99000000000001</v>
@@ -1020,13 +1020,13 @@
         <v>7.03</v>
       </c>
       <c r="I16">
-        <v>11.95862997379352</v>
+        <v>12.81281782906448</v>
       </c>
       <c r="J16">
-        <v>253.1243344452961</v>
+        <v>278.3228761757896</v>
       </c>
       <c r="K16">
-        <v>4.724409448818897</v>
+        <v>4.603580562659847</v>
       </c>
     </row>
     <row r="17">
@@ -1049,7 +1049,7 @@
         <v>1569439</v>
       </c>
       <c r="E17">
-        <v>3934</v>
+        <v>4774</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -1064,10 +1064,10 @@
         <v>5.097362815630299</v>
       </c>
       <c r="J17">
-        <v>2506.628164586199</v>
+        <v>3041.851260227381</v>
       </c>
       <c r="K17">
-        <v>0.2033553634977122</v>
+        <v>0.1675743611227482</v>
       </c>
     </row>
     <row r="18">
@@ -1090,10 +1090,10 @@
         <v>3323929</v>
       </c>
       <c r="E18">
-        <v>1987</v>
+        <v>2070</v>
       </c>
       <c r="F18">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="G18">
         <v>72.17</v>
@@ -1102,13 +1102,13 @@
         <v>4.87</v>
       </c>
       <c r="I18">
-        <v>25.8729954821538</v>
+        <v>29.48318089826828</v>
       </c>
       <c r="J18">
-        <v>597.7865351516233</v>
+        <v>622.7569842797484</v>
       </c>
       <c r="K18">
-        <v>4.328132863613487</v>
+        <v>4.734299516908213</v>
       </c>
     </row>
     <row r="19">
@@ -1131,10 +1131,10 @@
         <v>9485386</v>
       </c>
       <c r="E19">
-        <v>19255</v>
+        <v>22052</v>
       </c>
       <c r="F19">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="G19">
         <v>47.57</v>
@@ -1143,13 +1143,13 @@
         <v>3.13</v>
       </c>
       <c r="I19">
-        <v>11.80763755950469</v>
+        <v>13.28359225444278</v>
       </c>
       <c r="J19">
-        <v>2029.964832216633</v>
+        <v>2324.839495198192</v>
       </c>
       <c r="K19">
-        <v>0.5816670994546871</v>
+        <v>0.5713767458733902</v>
       </c>
     </row>
     <row r="20">
@@ -1172,10 +1172,10 @@
         <v>11353142</v>
       </c>
       <c r="E20">
-        <v>1886</v>
+        <v>2437</v>
       </c>
       <c r="F20">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="G20">
         <v>66.12</v>
@@ -1184,13 +1184,13 @@
         <v>5.49</v>
       </c>
       <c r="I20">
-        <v>8.015402256045066</v>
+        <v>10.04127315592459</v>
       </c>
       <c r="J20">
-        <v>166.1214137901208</v>
+        <v>214.6542340437564</v>
       </c>
       <c r="K20">
-        <v>4.825026511134676</v>
+        <v>4.677882642593353</v>
       </c>
     </row>
     <row r="21">
@@ -1213,10 +1213,10 @@
         <v>209469333</v>
       </c>
       <c r="E21">
-        <v>125218</v>
+        <v>155939</v>
       </c>
       <c r="F21">
-        <v>8536</v>
+        <v>10627</v>
       </c>
       <c r="G21">
         <v>66.42</v>
@@ -1225,13 +1225,13 @@
         <v>6.86</v>
       </c>
       <c r="I21">
-        <v>40.75059521958759</v>
+        <v>50.73296337846266</v>
       </c>
       <c r="J21">
-        <v>597.7867891525677</v>
+        <v>744.4478758138787</v>
       </c>
       <c r="K21">
-        <v>6.816911306681147</v>
+        <v>6.814844266027101</v>
       </c>
     </row>
     <row r="22">
@@ -1336,7 +1336,7 @@
         <v>4666377</v>
       </c>
       <c r="E24">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>20.14410751638798</v>
+        <v>30.64475930684555</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -1377,10 +1377,10 @@
         <v>37058856</v>
       </c>
       <c r="E25">
-        <v>63496</v>
+        <v>67702</v>
       </c>
       <c r="F25">
-        <v>4232</v>
+        <v>4693</v>
       </c>
       <c r="G25">
         <v>83.47</v>
@@ -1389,13 +1389,13 @@
         <v>9.15</v>
       </c>
       <c r="I25">
-        <v>114.1967253387422</v>
+        <v>126.636396978903</v>
       </c>
       <c r="J25">
-        <v>1713.382625734588</v>
+        <v>1826.877764386467</v>
       </c>
       <c r="K25">
-        <v>6.664986770820209</v>
+        <v>6.931848394434434</v>
       </c>
     </row>
     <row r="26">
@@ -1418,10 +1418,10 @@
         <v>8516543</v>
       </c>
       <c r="E26">
-        <v>29977</v>
+        <v>30168</v>
       </c>
       <c r="F26">
-        <v>1504</v>
+        <v>1531</v>
       </c>
       <c r="G26">
         <v>87.87</v>
@@ -1430,13 +1430,13 @@
         <v>9.029999999999999</v>
       </c>
       <c r="I26">
-        <v>176.5974762294983</v>
+        <v>179.7677766671289</v>
       </c>
       <c r="J26">
-        <v>3519.855415513079</v>
+        <v>3542.282355645947</v>
       </c>
       <c r="K26">
-        <v>5.017179837875705</v>
+        <v>5.074913815963935</v>
       </c>
     </row>
     <row r="27">
@@ -1459,10 +1459,10 @@
         <v>18729160</v>
       </c>
       <c r="E27">
-        <v>23048</v>
+        <v>27219</v>
       </c>
       <c r="F27">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="G27">
         <v>79.47</v>
@@ -1471,13 +1471,13 @@
         <v>7.84</v>
       </c>
       <c r="I27">
-        <v>15.00334238161242</v>
+        <v>16.23137396444902</v>
       </c>
       <c r="J27">
-        <v>1230.594431357306</v>
+        <v>1453.295289270848</v>
       </c>
       <c r="K27">
-        <v>1.219194724054148</v>
+        <v>1.116866894448731</v>
       </c>
     </row>
     <row r="28">
@@ -1500,7 +1500,7 @@
         <v>1392730000</v>
       </c>
       <c r="E28">
-        <v>83970</v>
+        <v>83991</v>
       </c>
       <c r="F28">
         <v>4637</v>
@@ -1515,10 +1515,10 @@
         <v>3.329432122521953</v>
       </c>
       <c r="J28">
-        <v>60.29165739231581</v>
+        <v>60.30673569177084</v>
       </c>
       <c r="K28">
-        <v>5.522210313207098</v>
+        <v>5.520829612696598</v>
       </c>
     </row>
     <row r="29">
@@ -1541,10 +1541,10 @@
         <v>25069229</v>
       </c>
       <c r="E29">
-        <v>1516</v>
+        <v>1667</v>
       </c>
       <c r="F29">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G29">
         <v>69.58</v>
@@ -1553,13 +1553,13 @@
         <v>3.93</v>
       </c>
       <c r="I29">
-        <v>0.7180117106912223</v>
+        <v>0.8376803291397593</v>
       </c>
       <c r="J29">
-        <v>60.47254185599405</v>
+        <v>66.49586231790374</v>
       </c>
       <c r="K29">
-        <v>1.187335092348285</v>
+        <v>1.259748050389922</v>
       </c>
     </row>
     <row r="30">
@@ -1582,7 +1582,7 @@
         <v>25216237</v>
       </c>
       <c r="E30">
-        <v>2265</v>
+        <v>2274</v>
       </c>
       <c r="F30">
         <v>108</v>
@@ -1597,10 +1597,10 @@
         <v>4.282954669247438</v>
       </c>
       <c r="J30">
-        <v>89.82307709116154</v>
+        <v>90.17998998026549</v>
       </c>
       <c r="K30">
-        <v>4.768211920529802</v>
+        <v>4.749340369393139</v>
       </c>
     </row>
     <row r="31">
@@ -1623,10 +1623,10 @@
         <v>84068091</v>
       </c>
       <c r="E31">
-        <v>863</v>
+        <v>991</v>
       </c>
       <c r="F31">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G31">
         <v>47.33</v>
@@ -1635,13 +1635,13 @@
         <v>1.61</v>
       </c>
       <c r="I31">
-        <v>0.4282243068895188</v>
+        <v>0.4876999050686188</v>
       </c>
       <c r="J31">
-        <v>10.26548824571263</v>
+        <v>11.78806355909759</v>
       </c>
       <c r="K31">
-        <v>4.171494785631518</v>
+        <v>4.137235116044399</v>
       </c>
     </row>
     <row r="32">
@@ -1664,7 +1664,7 @@
         <v>5244363</v>
       </c>
       <c r="E32">
-        <v>264</v>
+        <v>287</v>
       </c>
       <c r="F32">
         <v>10</v>
@@ -1679,10 +1679,10 @@
         <v>1.906809273118585</v>
       </c>
       <c r="J32">
-        <v>50.33976481033064</v>
+        <v>54.72542613850338</v>
       </c>
       <c r="K32">
-        <v>3.787878787878788</v>
+        <v>3.484320557491289</v>
       </c>
     </row>
     <row r="33">
@@ -1705,10 +1705,10 @@
         <v>49648685</v>
       </c>
       <c r="E33">
-        <v>8959</v>
+        <v>10495</v>
       </c>
       <c r="F33">
-        <v>397</v>
+        <v>445</v>
       </c>
       <c r="G33">
         <v>58.53</v>
@@ -1717,13 +1717,13 @@
         <v>6.67</v>
       </c>
       <c r="I33">
-        <v>7.996183584721328</v>
+        <v>8.96297656221912</v>
       </c>
       <c r="J33">
-        <v>180.4478809458901</v>
+        <v>211.3852562258195</v>
       </c>
       <c r="K33">
-        <v>4.431298135952674</v>
+        <v>4.240114340161981</v>
       </c>
     </row>
     <row r="34">
@@ -1746,7 +1746,7 @@
         <v>832322</v>
       </c>
       <c r="E34">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1761,10 +1761,10 @@
         <v>1.201458089537463</v>
       </c>
       <c r="J34">
-        <v>9.611664716299702</v>
+        <v>13.21603898491209</v>
       </c>
       <c r="K34">
-        <v>12.5</v>
+        <v>9.090909090909092</v>
       </c>
     </row>
     <row r="35">
@@ -1787,7 +1787,7 @@
         <v>543767</v>
       </c>
       <c r="E35">
-        <v>191</v>
+        <v>236</v>
       </c>
       <c r="F35">
         <v>2</v>
@@ -1802,10 +1802,10 @@
         <v>3.6780459277595</v>
       </c>
       <c r="J35">
-        <v>351.2533861010323</v>
+        <v>434.009419475621</v>
       </c>
       <c r="K35">
-        <v>1.047120418848168</v>
+        <v>0.847457627118644</v>
       </c>
     </row>
     <row r="36">
@@ -1828,7 +1828,7 @@
         <v>4999441</v>
       </c>
       <c r="E36">
-        <v>761</v>
+        <v>780</v>
       </c>
       <c r="F36">
         <v>6</v>
@@ -1843,10 +1843,10 @@
         <v>1.200134175000765</v>
       </c>
       <c r="J36">
-        <v>152.217017862597</v>
+        <v>156.0174427500995</v>
       </c>
       <c r="K36">
-        <v>0.7884362680683311</v>
+        <v>0.7692307692307693</v>
       </c>
     </row>
     <row r="37">
@@ -1869,10 +1869,10 @@
         <v>11338138</v>
       </c>
       <c r="E37">
-        <v>1703</v>
+        <v>1754</v>
       </c>
       <c r="F37">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G37">
         <v>28.25</v>
@@ -1881,13 +1881,13 @@
         <v>3.31</v>
       </c>
       <c r="I37">
-        <v>6.085655334235656</v>
+        <v>6.526644851209255</v>
       </c>
       <c r="J37">
-        <v>150.2010294812076</v>
+        <v>154.6991225543383</v>
       </c>
       <c r="K37">
-        <v>4.051673517322373</v>
+        <v>4.218928164196123</v>
       </c>
     </row>
     <row r="38">
@@ -1910,7 +1910,7 @@
         <v>1189265</v>
       </c>
       <c r="E38">
-        <v>883</v>
+        <v>892</v>
       </c>
       <c r="F38">
         <v>21</v>
@@ -1925,10 +1925,10 @@
         <v>17.65796521380853</v>
       </c>
       <c r="J38">
-        <v>742.47539446633</v>
+        <v>750.0430938436766</v>
       </c>
       <c r="K38">
-        <v>2.378255945639864</v>
+        <v>2.354260089686099</v>
       </c>
     </row>
     <row r="39">
@@ -1951,10 +1951,10 @@
         <v>10625695</v>
       </c>
       <c r="E39">
-        <v>7974</v>
+        <v>8095</v>
       </c>
       <c r="F39">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="G39">
         <v>83.09</v>
@@ -1963,13 +1963,13 @@
         <v>7.62</v>
       </c>
       <c r="I39">
-        <v>24.65721065774991</v>
+        <v>25.97477153259152</v>
       </c>
       <c r="J39">
-        <v>750.4450297133504</v>
+        <v>761.8325201316244</v>
       </c>
       <c r="K39">
-        <v>3.285678454978681</v>
+        <v>3.409512044471896</v>
       </c>
     </row>
     <row r="40">
@@ -1992,10 +1992,10 @@
         <v>82927922</v>
       </c>
       <c r="E40">
-        <v>166091</v>
+        <v>169218</v>
       </c>
       <c r="F40">
-        <v>7119</v>
+        <v>7395</v>
       </c>
       <c r="G40">
         <v>85.03</v>
@@ -2004,13 +2004,13 @@
         <v>8.609999999999999</v>
       </c>
       <c r="I40">
-        <v>85.8456335129198</v>
+        <v>89.1738249512631</v>
       </c>
       <c r="J40">
-        <v>2002.835667340127</v>
+        <v>2040.543111643386</v>
       </c>
       <c r="K40">
-        <v>4.286204550517487</v>
+        <v>4.370102471368295</v>
       </c>
     </row>
     <row r="41">
@@ -2033,7 +2033,7 @@
         <v>958920</v>
       </c>
       <c r="E41">
-        <v>1120</v>
+        <v>1189</v>
       </c>
       <c r="F41">
         <v>3</v>
@@ -2048,10 +2048,10 @@
         <v>3.128519584532599</v>
       </c>
       <c r="J41">
-        <v>1167.98064489217</v>
+        <v>1239.93659533642</v>
       </c>
       <c r="K41">
-        <v>0.2678571428571428</v>
+        <v>0.2523128679562658</v>
       </c>
     </row>
     <row r="42">
@@ -2074,10 +2074,10 @@
         <v>5797446</v>
       </c>
       <c r="E42">
-        <v>9983</v>
+        <v>10319</v>
       </c>
       <c r="F42">
-        <v>506</v>
+        <v>526</v>
       </c>
       <c r="G42">
         <v>89.64</v>
@@ -2086,13 +2086,13 @@
         <v>9.220000000000001</v>
       </c>
       <c r="I42">
-        <v>87.27981252434262</v>
+        <v>90.72960748577908</v>
       </c>
       <c r="J42">
-        <v>1721.965155001012</v>
+        <v>1779.921710353145</v>
       </c>
       <c r="K42">
-        <v>5.068616648302114</v>
+        <v>5.097393158251768</v>
       </c>
     </row>
     <row r="43">
@@ -2115,10 +2115,10 @@
         <v>10627165</v>
       </c>
       <c r="E43">
-        <v>8807</v>
+        <v>9882</v>
       </c>
       <c r="F43">
-        <v>362</v>
+        <v>385</v>
       </c>
       <c r="G43">
         <v>73.23999999999999</v>
@@ -2127,13 +2127,13 @@
         <v>6.66</v>
       </c>
       <c r="I43">
-        <v>34.06364726622763</v>
+        <v>36.22791214778353</v>
       </c>
       <c r="J43">
-        <v>828.7252526896872</v>
+        <v>929.8811112841477</v>
       </c>
       <c r="K43">
-        <v>4.110366753718632</v>
+        <v>3.895972475207448</v>
       </c>
     </row>
     <row r="44">
@@ -2156,10 +2156,10 @@
         <v>42228429</v>
       </c>
       <c r="E44">
-        <v>4997</v>
+        <v>5558</v>
       </c>
       <c r="F44">
-        <v>476</v>
+        <v>494</v>
       </c>
       <c r="G44">
         <v>57.17</v>
@@ -2168,13 +2168,13 @@
         <v>3.56</v>
       </c>
       <c r="I44">
-        <v>11.27202719286574</v>
+        <v>11.69828032200772</v>
       </c>
       <c r="J44">
-        <v>118.3326047956934</v>
+        <v>131.6174939872852</v>
       </c>
       <c r="K44">
-        <v>9.525715429257554</v>
+        <v>8.888089240734077</v>
       </c>
     </row>
     <row r="45">
@@ -2197,10 +2197,10 @@
         <v>17084357</v>
       </c>
       <c r="E45">
-        <v>29420</v>
+        <v>29071</v>
       </c>
       <c r="F45">
-        <v>1618</v>
+        <v>1717</v>
       </c>
       <c r="G45">
         <v>66.36</v>
@@ -2209,13 +2209,13 @@
         <v>6.02</v>
       </c>
       <c r="I45">
-        <v>94.70652012247227</v>
+        <v>100.5012948394839</v>
       </c>
       <c r="J45">
-        <v>1722.043153277586</v>
+        <v>1701.615109073171</v>
       </c>
       <c r="K45">
-        <v>5.499660095173351</v>
+        <v>5.906229575865983</v>
       </c>
     </row>
     <row r="46">
@@ -2238,10 +2238,10 @@
         <v>98423595</v>
       </c>
       <c r="E46">
-        <v>7588</v>
+        <v>8964</v>
       </c>
       <c r="F46">
-        <v>469</v>
+        <v>514</v>
       </c>
       <c r="G46">
         <v>44.22</v>
@@ -2250,13 +2250,13 @@
         <v>3.36</v>
       </c>
       <c r="I46">
-        <v>4.765117551335124</v>
+        <v>5.222324992294785</v>
       </c>
       <c r="J46">
-        <v>77.09533471115336</v>
+        <v>91.07572223916429</v>
       </c>
       <c r="K46">
-        <v>6.180811808118081</v>
+        <v>5.734047300312361</v>
       </c>
     </row>
     <row r="47">
@@ -2311,10 +2311,10 @@
         <v>46723749</v>
       </c>
       <c r="E48">
-        <v>220325</v>
+        <v>223578</v>
       </c>
       <c r="F48">
-        <v>25857</v>
+        <v>26478</v>
       </c>
       <c r="G48">
         <v>81.31</v>
@@ -2323,13 +2323,13 @@
         <v>8.08</v>
       </c>
       <c r="I48">
-        <v>553.4016544776833</v>
+        <v>566.6925400185675</v>
       </c>
       <c r="J48">
-        <v>4715.482056031077</v>
+        <v>4785.104037777448</v>
       </c>
       <c r="K48">
-        <v>11.73584477476455</v>
+        <v>11.84284679172369</v>
       </c>
     </row>
     <row r="49">
@@ -2352,10 +2352,10 @@
         <v>1320884</v>
       </c>
       <c r="E49">
-        <v>1713</v>
+        <v>1733</v>
       </c>
       <c r="F49">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G49">
         <v>86.45</v>
@@ -2364,13 +2364,13 @@
         <v>7.79</v>
       </c>
       <c r="I49">
-        <v>41.63878130100751</v>
+        <v>45.42412505564455</v>
       </c>
       <c r="J49">
-        <v>1296.858770338652</v>
+        <v>1312.0001453572</v>
       </c>
       <c r="K49">
-        <v>3.210741389375365</v>
+        <v>3.462204270051933</v>
       </c>
     </row>
     <row r="50">
@@ -2393,10 +2393,10 @@
         <v>109224559</v>
       </c>
       <c r="E50">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="F50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G50">
         <v>49.66</v>
@@ -2405,13 +2405,13 @@
         <v>3.42</v>
       </c>
       <c r="I50">
-        <v>0.03662180041395269</v>
+        <v>0.04577725051744086</v>
       </c>
       <c r="J50">
-        <v>1.483182916765084</v>
+        <v>1.922644521732516</v>
       </c>
       <c r="K50">
-        <v>2.469135802469136</v>
+        <v>2.380952380952381</v>
       </c>
     </row>
     <row r="51">
@@ -2434,10 +2434,10 @@
         <v>5518050</v>
       </c>
       <c r="E51">
-        <v>5573</v>
+        <v>5880</v>
       </c>
       <c r="F51">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="G51">
         <v>91.08</v>
@@ -2446,13 +2446,13 @@
         <v>9.029999999999999</v>
       </c>
       <c r="I51">
-        <v>45.6683067387936</v>
+        <v>48.02421145150914</v>
       </c>
       <c r="J51">
-        <v>1009.958227997209</v>
+        <v>1065.593823905184</v>
       </c>
       <c r="K51">
-        <v>4.521801543154495</v>
+        <v>4.506802721088436</v>
       </c>
     </row>
     <row r="52">
@@ -2475,10 +2475,10 @@
         <v>66987244</v>
       </c>
       <c r="E52">
-        <v>137150</v>
+        <v>138854</v>
       </c>
       <c r="F52">
-        <v>25809</v>
+        <v>26310</v>
       </c>
       <c r="G52">
         <v>77.76000000000001</v>
@@ -2487,13 +2487,13 @@
         <v>7.8</v>
       </c>
       <c r="I52">
-        <v>385.2823083750094</v>
+        <v>392.7613442344336</v>
       </c>
       <c r="J52">
-        <v>2047.404726786491</v>
+        <v>2072.842405637706</v>
       </c>
       <c r="K52">
-        <v>18.81808239154211</v>
+        <v>18.94795972748354</v>
       </c>
     </row>
     <row r="53">
@@ -2516,7 +2516,7 @@
         <v>2119275</v>
       </c>
       <c r="E53">
-        <v>439</v>
+        <v>661</v>
       </c>
       <c r="F53">
         <v>8</v>
@@ -2531,10 +2531,10 @@
         <v>3.77487584197426</v>
       </c>
       <c r="J53">
-        <v>207.1463118283375</v>
+        <v>311.8991164431233</v>
       </c>
       <c r="K53">
-        <v>1.822323462414579</v>
+        <v>1.210287443267776</v>
       </c>
     </row>
     <row r="54">
@@ -2557,10 +2557,10 @@
         <v>66488991</v>
       </c>
       <c r="E54">
-        <v>201201</v>
+        <v>215260</v>
       </c>
       <c r="F54">
-        <v>30076</v>
+        <v>31587</v>
       </c>
       <c r="G54">
         <v>77.73999999999999</v>
@@ -2569,13 +2569,13 @@
         <v>8.529999999999999</v>
       </c>
       <c r="I54">
-        <v>452.3455619893525</v>
+        <v>475.0711286925681</v>
       </c>
       <c r="J54">
-        <v>3026.079911484896</v>
+        <v>3237.528450386621</v>
       </c>
       <c r="K54">
-        <v>14.94823584375823</v>
+        <v>14.67388274644616</v>
       </c>
     </row>
     <row r="55">
@@ -2598,10 +2598,10 @@
         <v>3731000</v>
       </c>
       <c r="E55">
-        <v>610</v>
+        <v>626</v>
       </c>
       <c r="F55">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G55">
         <v>72.23999999999999</v>
@@ -2610,13 +2610,13 @@
         <v>5.93</v>
       </c>
       <c r="I55">
-        <v>2.412221924417046</v>
+        <v>2.680246582685607</v>
       </c>
       <c r="J55">
-        <v>163.495041543822</v>
+        <v>167.783436076119</v>
       </c>
       <c r="K55">
-        <v>1.475409836065574</v>
+        <v>1.597444089456869</v>
       </c>
     </row>
     <row r="56">
@@ -2639,10 +2639,10 @@
         <v>29767108</v>
       </c>
       <c r="E56">
-        <v>3091</v>
+        <v>4263</v>
       </c>
       <c r="F56">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G56">
         <v>82.05</v>
@@ -2651,13 +2651,13 @@
         <v>6.69</v>
       </c>
       <c r="I56">
-        <v>0.6046942820243068</v>
+        <v>0.7390707891408195</v>
       </c>
       <c r="J56">
-        <v>103.8394458742851</v>
+        <v>143.2117624594233</v>
       </c>
       <c r="K56">
-        <v>0.5823358136525397</v>
+        <v>0.5160684963640628</v>
       </c>
     </row>
     <row r="57">
@@ -2680,7 +2680,7 @@
         <v>12414318</v>
       </c>
       <c r="E57">
-        <v>1856</v>
+        <v>2042</v>
       </c>
       <c r="F57">
         <v>11</v>
@@ -2695,10 +2695,10 @@
         <v>0.8860736449638232</v>
       </c>
       <c r="J57">
-        <v>149.5047895502596</v>
+        <v>164.4874893651024</v>
       </c>
       <c r="K57">
-        <v>0.5926724137931034</v>
+        <v>0.5386875612144956</v>
       </c>
     </row>
     <row r="58">
@@ -2721,7 +2721,7 @@
         <v>2280102</v>
       </c>
       <c r="E58">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -2736,10 +2736,10 @@
         <v>0.4385768706838554</v>
       </c>
       <c r="J58">
-        <v>7.455806801625542</v>
+        <v>8.771537413677107</v>
       </c>
       <c r="K58">
-        <v>5.88235294117647</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59">
@@ -2762,10 +2762,10 @@
         <v>1874309</v>
       </c>
       <c r="E59">
-        <v>475</v>
+        <v>641</v>
       </c>
       <c r="F59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G59">
         <v>69.91</v>
@@ -2774,13 +2774,13 @@
         <v>1.98</v>
       </c>
       <c r="I59">
-        <v>1.067059913813571</v>
+        <v>1.600589870720356</v>
       </c>
       <c r="J59">
-        <v>253.4267295307231</v>
+        <v>341.9927023772494</v>
       </c>
       <c r="K59">
-        <v>0.4210526315789473</v>
+        <v>0.46801872074883</v>
       </c>
     </row>
     <row r="60">
@@ -2844,10 +2844,10 @@
         <v>10727668</v>
       </c>
       <c r="E61">
-        <v>2663</v>
+        <v>2710</v>
       </c>
       <c r="F61">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G61">
         <v>69.11</v>
@@ -2856,13 +2856,13 @@
         <v>7.29</v>
       </c>
       <c r="I61">
-        <v>13.70288491403723</v>
+        <v>14.07575253074573</v>
       </c>
       <c r="J61">
-        <v>248.2366158236814</v>
+        <v>252.6178103200062</v>
       </c>
       <c r="K61">
-        <v>5.52009012392039</v>
+        <v>5.571955719557196</v>
       </c>
     </row>
     <row r="62">
@@ -2885,10 +2885,10 @@
         <v>17247807</v>
       </c>
       <c r="E62">
-        <v>798</v>
+        <v>967</v>
       </c>
       <c r="F62">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G62">
         <v>60.67</v>
@@ -2897,13 +2897,13 @@
         <v>5.86</v>
       </c>
       <c r="I62">
-        <v>1.217546091511808</v>
+        <v>1.391481247442066</v>
       </c>
       <c r="J62">
-        <v>46.26675147744869</v>
+        <v>56.06509859485325</v>
       </c>
       <c r="K62">
-        <v>2.631578947368421</v>
+        <v>2.481902792140641</v>
       </c>
     </row>
     <row r="63">
@@ -2926,7 +2926,7 @@
         <v>779004</v>
       </c>
       <c r="E63">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F63">
         <v>10</v>
@@ -2941,10 +2941,10 @@
         <v>12.83690456018198</v>
       </c>
       <c r="J63">
-        <v>119.3832124096924</v>
+        <v>124.5179742337652</v>
       </c>
       <c r="K63">
-        <v>10.75268817204301</v>
+        <v>10.30927835051546</v>
       </c>
     </row>
     <row r="64">
@@ -2967,10 +2967,10 @@
         <v>9587522</v>
       </c>
       <c r="E64">
-        <v>1461</v>
+        <v>1830</v>
       </c>
       <c r="F64">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="G64">
         <v>56.25</v>
@@ -2979,13 +2979,13 @@
         <v>5.72</v>
       </c>
       <c r="I64">
-        <v>10.32592154677715</v>
+        <v>11.26464168739326</v>
       </c>
       <c r="J64">
-        <v>152.3855694933477</v>
+        <v>190.873095258608</v>
       </c>
       <c r="K64">
-        <v>6.776180698151951</v>
+        <v>5.901639344262295</v>
       </c>
     </row>
     <row r="65">
@@ -3008,10 +3008,10 @@
         <v>4089400</v>
       </c>
       <c r="E65">
-        <v>2119</v>
+        <v>2176</v>
       </c>
       <c r="F65">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G65">
         <v>70.41</v>
@@ -3020,13 +3020,13 @@
         <v>6.63</v>
       </c>
       <c r="I65">
-        <v>20.78544529759867</v>
+        <v>21.27451459871864</v>
       </c>
       <c r="J65">
-        <v>518.1689245366068</v>
+        <v>532.107399618526</v>
       </c>
       <c r="K65">
-        <v>4.011326097215668</v>
+        <v>3.998161764705882</v>
       </c>
     </row>
     <row r="66">
@@ -3049,7 +3049,7 @@
         <v>11123176</v>
       </c>
       <c r="E66">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="F66">
         <v>12</v>
@@ -3064,10 +3064,10 @@
         <v>1.078828564791207</v>
       </c>
       <c r="J66">
-        <v>9.709457083120864</v>
+        <v>13.57525944028936</v>
       </c>
       <c r="K66">
-        <v>11.11111111111111</v>
+        <v>7.947019867549669</v>
       </c>
     </row>
     <row r="67">
@@ -3090,10 +3090,10 @@
         <v>9768785</v>
       </c>
       <c r="E67">
-        <v>3150</v>
+        <v>3263</v>
       </c>
       <c r="F67">
-        <v>383</v>
+        <v>413</v>
       </c>
       <c r="G67">
         <v>70.98999999999999</v>
@@ -3102,13 +3102,13 @@
         <v>6.64</v>
       </c>
       <c r="I67">
-        <v>39.20651339956812</v>
+        <v>42.27751967107476</v>
       </c>
       <c r="J67">
-        <v>322.4556585081972</v>
+        <v>334.0231154642056</v>
       </c>
       <c r="K67">
-        <v>12.15873015873016</v>
+        <v>12.65706405148636</v>
       </c>
     </row>
     <row r="68">
@@ -3131,10 +3131,10 @@
         <v>267663435</v>
       </c>
       <c r="E68">
-        <v>12438</v>
+        <v>13645</v>
       </c>
       <c r="F68">
-        <v>895</v>
+        <v>959</v>
       </c>
       <c r="G68">
         <v>60.07</v>
@@ -3143,13 +3143,13 @@
         <v>6.39</v>
       </c>
       <c r="I68">
-        <v>3.343751454134929</v>
+        <v>3.582857703369158</v>
       </c>
       <c r="J68">
-        <v>46.4688051246148</v>
+        <v>50.97819954376659</v>
       </c>
       <c r="K68">
-        <v>7.195690625502491</v>
+        <v>7.028215463539758</v>
       </c>
     </row>
     <row r="69">
@@ -3172,10 +3172,10 @@
         <v>1352617328</v>
       </c>
       <c r="E69">
-        <v>52952</v>
+        <v>62939</v>
       </c>
       <c r="F69">
-        <v>1783</v>
+        <v>2109</v>
       </c>
       <c r="G69">
         <v>57.06</v>
@@ -3184,13 +3184,13 @@
         <v>7.23</v>
       </c>
       <c r="I69">
-        <v>1.318185094254537</v>
+        <v>1.559199306664508</v>
       </c>
       <c r="J69">
-        <v>39.14780544641965</v>
+        <v>46.53126845052513</v>
       </c>
       <c r="K69">
-        <v>3.367200483456716</v>
+        <v>3.350863534533437</v>
       </c>
     </row>
     <row r="70">
@@ -3213,10 +3213,10 @@
         <v>4853506</v>
       </c>
       <c r="E70">
-        <v>22248</v>
+        <v>22760</v>
       </c>
       <c r="F70">
-        <v>1375</v>
+        <v>1446</v>
       </c>
       <c r="G70">
         <v>85.92</v>
@@ -3225,13 +3225,13 @@
         <v>9.15</v>
       </c>
       <c r="I70">
-        <v>283.3003606053026</v>
+        <v>297.928961043831</v>
       </c>
       <c r="J70">
-        <v>4583.902852906745</v>
+        <v>4689.393605364864</v>
       </c>
       <c r="K70">
-        <v>6.180330816253147</v>
+        <v>6.353251318101933</v>
       </c>
     </row>
     <row r="71">
@@ -3254,10 +3254,10 @@
         <v>81800269</v>
       </c>
       <c r="E71">
-        <v>101650</v>
+        <v>106220</v>
       </c>
       <c r="F71">
-        <v>6418</v>
+        <v>6589</v>
       </c>
       <c r="G71">
         <v>34.88</v>
@@ -3266,13 +3266,13 @@
         <v>2.45</v>
       </c>
       <c r="I71">
-        <v>78.45939968730421</v>
+        <v>80.54985736049352</v>
       </c>
       <c r="J71">
-        <v>1242.660950173648</v>
+        <v>1298.528737112099</v>
       </c>
       <c r="K71">
-        <v>6.313821938022627</v>
+        <v>6.203163246093014</v>
       </c>
     </row>
     <row r="72">
@@ -3295,10 +3295,10 @@
         <v>38433600</v>
       </c>
       <c r="E72">
-        <v>2480</v>
+        <v>2679</v>
       </c>
       <c r="F72">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G72">
         <v>45.97</v>
@@ -3307,13 +3307,13 @@
         <v>4.09</v>
       </c>
       <c r="I72">
-        <v>2.653927813163482</v>
+        <v>2.784022313808751</v>
       </c>
       <c r="J72">
-        <v>64.52687232005329</v>
+        <v>69.70463344573498</v>
       </c>
       <c r="K72">
-        <v>4.112903225806452</v>
+        <v>3.994027622247107</v>
       </c>
     </row>
     <row r="73">
@@ -3336,7 +3336,7 @@
         <v>353574</v>
       </c>
       <c r="E73">
-        <v>1799</v>
+        <v>1801</v>
       </c>
       <c r="F73">
         <v>10</v>
@@ -3351,10 +3351,10 @@
         <v>28.28262259102762</v>
       </c>
       <c r="J73">
-        <v>5088.043804125869</v>
+        <v>5093.700328644074</v>
       </c>
       <c r="K73">
-        <v>0.5558643690939411</v>
+        <v>0.5552470849528041</v>
       </c>
     </row>
     <row r="74">
@@ -3377,10 +3377,10 @@
         <v>8883800</v>
       </c>
       <c r="E74">
-        <v>16310</v>
+        <v>16454</v>
       </c>
       <c r="F74">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="G74">
         <v>68.98999999999999</v>
@@ -3389,13 +3389,13 @@
         <v>7.79</v>
       </c>
       <c r="I74">
-        <v>26.90290191134424</v>
+        <v>27.80341745649384</v>
       </c>
       <c r="J74">
-        <v>1835.926067673743</v>
+        <v>1852.135347486436</v>
       </c>
       <c r="K74">
-        <v>1.465358675659105</v>
+        <v>1.501154734411085</v>
       </c>
     </row>
     <row r="75">
@@ -3418,10 +3418,10 @@
         <v>60431283</v>
       </c>
       <c r="E75">
-        <v>214457</v>
+        <v>218268</v>
       </c>
       <c r="F75">
-        <v>29684</v>
+        <v>30395</v>
       </c>
       <c r="G75">
         <v>73.73999999999999</v>
@@ -3430,13 +3430,13 @@
         <v>7.98</v>
       </c>
       <c r="I75">
-        <v>491.2025448806043</v>
+        <v>502.9679743850548</v>
       </c>
       <c r="J75">
-        <v>3548.774564326228</v>
+        <v>3611.837928378916</v>
       </c>
       <c r="K75">
-        <v>13.84146938547121</v>
+        <v>13.92554107794088</v>
       </c>
     </row>
     <row r="76">
@@ -3459,7 +3459,7 @@
         <v>2934855</v>
       </c>
       <c r="E76">
-        <v>478</v>
+        <v>498</v>
       </c>
       <c r="F76">
         <v>9</v>
@@ -3474,10 +3474,10 @@
         <v>3.066591024088072</v>
       </c>
       <c r="J76">
-        <v>162.8700566126776</v>
+        <v>169.6847033328734</v>
       </c>
       <c r="K76">
-        <v>1.882845188284519</v>
+        <v>1.80722891566265</v>
       </c>
     </row>
     <row r="77">
@@ -3500,7 +3500,7 @@
         <v>9956011</v>
       </c>
       <c r="E77">
-        <v>473</v>
+        <v>522</v>
       </c>
       <c r="F77">
         <v>9</v>
@@ -3515,10 +3515,10 @@
         <v>0.9039765022356845</v>
       </c>
       <c r="J77">
-        <v>47.50898728416431</v>
+        <v>52.43063712966971</v>
       </c>
       <c r="K77">
-        <v>1.902748414376321</v>
+        <v>1.724137931034483</v>
       </c>
     </row>
     <row r="78">
@@ -3541,10 +3541,10 @@
         <v>126529100</v>
       </c>
       <c r="E78">
-        <v>15463</v>
+        <v>15747</v>
       </c>
       <c r="F78">
-        <v>551</v>
+        <v>613</v>
       </c>
       <c r="G78">
         <v>70.56</v>
@@ -3553,13 +3553,13 @@
         <v>7.88</v>
       </c>
       <c r="I78">
-        <v>4.354729465395708</v>
+        <v>4.844735321756023</v>
       </c>
       <c r="J78">
-        <v>122.2090412403155</v>
+        <v>124.4535841952563</v>
       </c>
       <c r="K78">
-        <v>3.563344758455669</v>
+        <v>3.892804978726107</v>
       </c>
     </row>
     <row r="79">
@@ -3582,10 +3582,10 @@
         <v>18276499</v>
       </c>
       <c r="E79">
-        <v>4502</v>
+        <v>5036</v>
       </c>
       <c r="F79">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G79">
         <v>45.99</v>
@@ -3594,13 +3594,13 @@
         <v>3.06</v>
       </c>
       <c r="I79">
-        <v>1.641452227803585</v>
+        <v>1.696167302063705</v>
       </c>
       <c r="J79">
-        <v>246.327264319058</v>
+        <v>275.5451139739619</v>
       </c>
       <c r="K79">
-        <v>0.6663705019991115</v>
+        <v>0.6155679110405083</v>
       </c>
     </row>
     <row r="80">
@@ -3623,10 +3623,10 @@
         <v>51393010</v>
       </c>
       <c r="E80">
-        <v>582</v>
+        <v>649</v>
       </c>
       <c r="F80">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G80">
         <v>68.8</v>
@@ -3635,13 +3635,13 @@
         <v>5.11</v>
       </c>
       <c r="I80">
-        <v>0.505905375069489</v>
+        <v>0.5837369712340258</v>
       </c>
       <c r="J80">
-        <v>11.3244972419401</v>
+        <v>12.62817647769609</v>
       </c>
       <c r="K80">
-        <v>4.467353951890034</v>
+        <v>4.622496147919876</v>
       </c>
     </row>
     <row r="81">
@@ -3664,7 +3664,7 @@
         <v>6315800</v>
       </c>
       <c r="E81">
-        <v>895</v>
+        <v>1002</v>
       </c>
       <c r="F81">
         <v>12</v>
@@ -3679,10 +3679,10 @@
         <v>1.899996833338611</v>
       </c>
       <c r="J81">
-        <v>141.7080971531714</v>
+        <v>158.649735583774</v>
       </c>
       <c r="K81">
-        <v>1.340782122905028</v>
+        <v>1.197604790419162</v>
       </c>
     </row>
     <row r="82">
@@ -3746,7 +3746,7 @@
         <v>51635256</v>
       </c>
       <c r="E83">
-        <v>10810</v>
+        <v>10874</v>
       </c>
       <c r="F83">
         <v>256</v>
@@ -3761,10 +3761,10 @@
         <v>4.957852828307852</v>
       </c>
       <c r="J83">
-        <v>209.3530823203433</v>
+        <v>210.5925455274202</v>
       </c>
       <c r="K83">
-        <v>2.368177613320999</v>
+        <v>2.354239470296119</v>
       </c>
     </row>
     <row r="84">
@@ -3787,10 +3787,10 @@
         <v>4137309</v>
       </c>
       <c r="E84">
-        <v>6289</v>
+        <v>7623</v>
       </c>
       <c r="F84">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G84">
         <v>66.39</v>
@@ -3799,13 +3799,13 @@
         <v>3.85</v>
       </c>
       <c r="I84">
-        <v>10.15152602815018</v>
+        <v>11.84344703284188</v>
       </c>
       <c r="J84">
-        <v>1520.070171215154</v>
+        <v>1842.501974109258</v>
       </c>
       <c r="K84">
-        <v>0.6678327238034664</v>
+        <v>0.642791551882461</v>
       </c>
     </row>
     <row r="85">
@@ -3869,10 +3869,10 @@
         <v>6848925</v>
       </c>
       <c r="E86">
-        <v>750</v>
+        <v>809</v>
       </c>
       <c r="F86">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G86">
         <v>66.99000000000001</v>
@@ -3881,13 +3881,13 @@
         <v>4.72</v>
       </c>
       <c r="I86">
-        <v>3.650207879338728</v>
+        <v>3.796216194512277</v>
       </c>
       <c r="J86">
-        <v>109.5062363801619</v>
+        <v>118.1207269754013</v>
       </c>
       <c r="K86">
-        <v>3.333333333333333</v>
+        <v>3.213844252163164</v>
       </c>
     </row>
     <row r="87">
@@ -3910,7 +3910,7 @@
         <v>4818977</v>
       </c>
       <c r="E87">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="F87">
         <v>20</v>
@@ -3925,10 +3925,10 @@
         <v>4.150258446969139</v>
       </c>
       <c r="J87">
-        <v>36.93730017802534</v>
+        <v>41.29507154734293</v>
       </c>
       <c r="K87">
-        <v>11.23595505617977</v>
+        <v>10.05025125628141</v>
       </c>
     </row>
     <row r="88">
@@ -3992,7 +3992,7 @@
         <v>21670000</v>
       </c>
       <c r="E89">
-        <v>797</v>
+        <v>847</v>
       </c>
       <c r="F89">
         <v>9</v>
@@ -4007,10 +4007,10 @@
         <v>0.4153207198892478</v>
       </c>
       <c r="J89">
-        <v>36.77895708352561</v>
+        <v>39.08629441624365</v>
       </c>
       <c r="K89">
-        <v>1.129234629861982</v>
+        <v>1.062573789846517</v>
       </c>
     </row>
     <row r="90">
@@ -4033,10 +4033,10 @@
         <v>2789533</v>
       </c>
       <c r="E90">
-        <v>1428</v>
+        <v>1444</v>
       </c>
       <c r="F90">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G90">
         <v>78.63</v>
@@ -4045,13 +4045,13 @@
         <v>7.41</v>
       </c>
       <c r="I90">
-        <v>17.20718127371141</v>
+        <v>17.92414716011605</v>
       </c>
       <c r="J90">
-        <v>511.9136428929144</v>
+        <v>517.6493699841515</v>
       </c>
       <c r="K90">
-        <v>3.361344537815126</v>
+        <v>3.462603878116344</v>
       </c>
     </row>
     <row r="91">
@@ -4074,10 +4074,10 @@
         <v>607728</v>
       </c>
       <c r="E91">
-        <v>3851</v>
+        <v>3877</v>
       </c>
       <c r="F91">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G91">
         <v>85.28</v>
@@ -4086,13 +4086,13 @@
         <v>8.81</v>
       </c>
       <c r="I91">
-        <v>161.2563515256825</v>
+        <v>166.1927704499381</v>
       </c>
       <c r="J91">
-        <v>6336.716425769423</v>
+        <v>6379.498723112972</v>
       </c>
       <c r="K91">
-        <v>2.544793560114256</v>
+        <v>2.605107041526954</v>
       </c>
     </row>
     <row r="92">
@@ -4115,10 +4115,10 @@
         <v>1926542</v>
       </c>
       <c r="E92">
-        <v>900</v>
+        <v>930</v>
       </c>
       <c r="F92">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G92">
         <v>81.38</v>
@@ -4127,13 +4127,13 @@
         <v>7.25</v>
       </c>
       <c r="I92">
-        <v>8.824100382965955</v>
+        <v>9.343165111375718</v>
       </c>
       <c r="J92">
-        <v>467.1582555687859</v>
+        <v>482.7301974210788</v>
       </c>
       <c r="K92">
-        <v>1.888888888888889</v>
+        <v>1.935483870967742</v>
       </c>
     </row>
     <row r="93">
@@ -4156,10 +4156,10 @@
         <v>36029138</v>
       </c>
       <c r="E93">
-        <v>5408</v>
+        <v>5910</v>
       </c>
       <c r="F93">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G93">
         <v>57.58</v>
@@ -4168,13 +4168,13 @@
         <v>4.87</v>
       </c>
       <c r="I93">
-        <v>5.079222267266012</v>
+        <v>5.162488206073651</v>
       </c>
       <c r="J93">
-        <v>150.1007323572382</v>
+        <v>164.0338994510498</v>
       </c>
       <c r="K93">
-        <v>3.38387573964497</v>
+        <v>3.147208121827411</v>
       </c>
     </row>
     <row r="94">
@@ -4197,10 +4197,10 @@
         <v>3545883</v>
       </c>
       <c r="E94">
-        <v>4476</v>
+        <v>4867</v>
       </c>
       <c r="F94">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="G94">
         <v>69.59</v>
@@ -4209,13 +4209,13 @@
         <v>5.94</v>
       </c>
       <c r="I94">
-        <v>40.32845979407668</v>
+        <v>45.40476941850591</v>
       </c>
       <c r="J94">
-        <v>1262.308993274736</v>
+        <v>1372.577719005393</v>
       </c>
       <c r="K94">
-        <v>3.194816800714924</v>
+        <v>3.307992603246353</v>
       </c>
     </row>
     <row r="95">
@@ -4238,7 +4238,7 @@
         <v>26262368</v>
       </c>
       <c r="E95">
-        <v>158</v>
+        <v>193</v>
       </c>
       <c r="F95">
         <v>0</v>
@@ -4253,7 +4253,7 @@
         <v>0</v>
       </c>
       <c r="J95">
-        <v>6.016213008667002</v>
+        <v>7.348918421979313</v>
       </c>
       <c r="K95">
         <v>0</v>
@@ -4279,10 +4279,10 @@
         <v>126190788</v>
       </c>
       <c r="E96">
-        <v>27634</v>
+        <v>33460</v>
       </c>
       <c r="F96">
-        <v>2704</v>
+        <v>3353</v>
       </c>
       <c r="G96">
         <v>51.03</v>
@@ -4291,13 +4291,13 @@
         <v>6.41</v>
       </c>
       <c r="I96">
-        <v>21.42787158124411</v>
+        <v>26.57087774109153</v>
       </c>
       <c r="J96">
-        <v>218.9858739926404</v>
+        <v>265.1540618004541</v>
       </c>
       <c r="K96">
-        <v>9.785047405370197</v>
+        <v>10.02092050209205</v>
       </c>
     </row>
     <row r="97">
@@ -4320,10 +4320,10 @@
         <v>2082958</v>
       </c>
       <c r="E97">
-        <v>1539</v>
+        <v>1622</v>
       </c>
       <c r="F97">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G97">
         <v>64.25999999999999</v>
@@ -4332,13 +4332,13 @@
         <v>5.57</v>
       </c>
       <c r="I97">
-        <v>42.24761132965715</v>
+        <v>43.68787080680455</v>
       </c>
       <c r="J97">
-        <v>738.8531117766178</v>
+        <v>778.7002906443626</v>
       </c>
       <c r="K97">
-        <v>5.71799870045484</v>
+        <v>5.61035758323058</v>
       </c>
     </row>
     <row r="98">
@@ -4361,10 +4361,10 @@
         <v>19077690</v>
       </c>
       <c r="E98">
-        <v>631</v>
+        <v>692</v>
       </c>
       <c r="F98">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G98">
         <v>61.73</v>
@@ -4373,13 +4373,13 @@
         <v>5.64</v>
       </c>
       <c r="I98">
-        <v>1.677351922586015</v>
+        <v>1.939438160490081</v>
       </c>
       <c r="J98">
-        <v>33.07528322349299</v>
+        <v>36.27273532592258</v>
       </c>
       <c r="K98">
-        <v>5.071315372424722</v>
+        <v>5.346820809248555</v>
       </c>
     </row>
     <row r="99">
@@ -4402,7 +4402,7 @@
         <v>53708395</v>
       </c>
       <c r="E99">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="F99">
         <v>6</v>
@@ -4417,10 +4417,10 @@
         <v>0.1117143791021869</v>
       </c>
       <c r="J99">
-        <v>3.016288235759046</v>
+        <v>3.314193246698212</v>
       </c>
       <c r="K99">
-        <v>3.703703703703703</v>
+        <v>3.370786516853932</v>
       </c>
     </row>
     <row r="100">
@@ -4443,7 +4443,7 @@
         <v>3170208</v>
       </c>
       <c r="E100">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -4458,7 +4458,7 @@
         <v>0</v>
       </c>
       <c r="J100">
-        <v>12.9329053487973</v>
+        <v>13.24834206462163</v>
       </c>
       <c r="K100">
         <v>0</v>
@@ -4484,7 +4484,7 @@
         <v>29495962</v>
       </c>
       <c r="E101">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F101">
         <v>0</v>
@@ -4499,7 +4499,7 @@
         <v>0</v>
       </c>
       <c r="J101">
-        <v>2.746138607040516</v>
+        <v>2.94955628163611</v>
       </c>
       <c r="K101">
         <v>0</v>
@@ -4607,7 +4607,7 @@
         <v>18143315</v>
       </c>
       <c r="E104">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F104">
         <v>3</v>
@@ -4622,10 +4622,10 @@
         <v>0.1653501578956216</v>
       </c>
       <c r="J104">
-        <v>2.370018929837243</v>
+        <v>3.08653628071827</v>
       </c>
       <c r="K104">
-        <v>6.976744186046512</v>
+        <v>5.357142857142857</v>
       </c>
     </row>
     <row r="105">
@@ -4648,10 +4648,10 @@
         <v>31528585</v>
       </c>
       <c r="E105">
-        <v>6428</v>
+        <v>6589</v>
       </c>
       <c r="F105">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G105">
         <v>53.11</v>
@@ -4660,13 +4660,13 @@
         <v>6.54</v>
       </c>
       <c r="I105">
-        <v>3.393745707268499</v>
+        <v>3.425462956869139</v>
       </c>
       <c r="J105">
-        <v>203.8784804329151</v>
+        <v>208.9849576186182</v>
       </c>
       <c r="K105">
-        <v>1.664592408214063</v>
+        <v>1.639095462133859</v>
       </c>
     </row>
     <row r="106">
@@ -4730,10 +4730,10 @@
         <v>22442948</v>
       </c>
       <c r="E107">
-        <v>770</v>
+        <v>815</v>
       </c>
       <c r="F107">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G107">
         <v>72.78999999999999</v>
@@ -4742,13 +4742,13 @@
         <v>3.76</v>
       </c>
       <c r="I107">
-        <v>1.693182196919941</v>
+        <v>2.005084180563088</v>
       </c>
       <c r="J107">
-        <v>34.30921820074617</v>
+        <v>36.31430238130927</v>
       </c>
       <c r="K107">
-        <v>4.935064935064935</v>
+        <v>5.521472392638037</v>
       </c>
     </row>
     <row r="108">
@@ -4771,10 +4771,10 @@
         <v>195874740</v>
       </c>
       <c r="E108">
-        <v>3145</v>
+        <v>4151</v>
       </c>
       <c r="F108">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="G108">
         <v>60.31</v>
@@ -4783,13 +4783,13 @@
         <v>4.44</v>
       </c>
       <c r="I108">
-        <v>0.5258462627697681</v>
+        <v>0.6534788508206826</v>
       </c>
       <c r="J108">
-        <v>16.05617957680505</v>
+        <v>21.19211491997386</v>
       </c>
       <c r="K108">
-        <v>3.275039745627981</v>
+        <v>3.083594314622983</v>
       </c>
     </row>
     <row r="109">
@@ -4853,10 +4853,10 @@
         <v>17231017</v>
       </c>
       <c r="E110">
-        <v>41319</v>
+        <v>42382</v>
       </c>
       <c r="F110">
-        <v>5204</v>
+        <v>5422</v>
       </c>
       <c r="G110">
         <v>88.72</v>
@@ -4865,13 +4865,13 @@
         <v>8.890000000000001</v>
       </c>
       <c r="I110">
-        <v>302.0135143503138</v>
+        <v>314.6651181413146</v>
       </c>
       <c r="J110">
-        <v>2397.943197432862</v>
+        <v>2459.634274633935</v>
       </c>
       <c r="K110">
-        <v>12.59469009414555</v>
+        <v>12.79316691048086</v>
       </c>
     </row>
     <row r="111">
@@ -4894,10 +4894,10 @@
         <v>5314336</v>
       </c>
       <c r="E111">
-        <v>7953</v>
+        <v>8069</v>
       </c>
       <c r="F111">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="G111">
         <v>92.40000000000001</v>
@@ -4906,13 +4906,13 @@
         <v>9.869999999999999</v>
       </c>
       <c r="I111">
-        <v>39.32758485726156</v>
+        <v>40.08026590716131</v>
       </c>
       <c r="J111">
-        <v>1496.518097463164</v>
+        <v>1518.345847910256</v>
       </c>
       <c r="K111">
-        <v>2.627939142461964</v>
+        <v>2.639732308836287</v>
       </c>
     </row>
     <row r="112">
@@ -4935,7 +4935,7 @@
         <v>28087871</v>
       </c>
       <c r="E112">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -4950,7 +4950,7 @@
         <v>0</v>
       </c>
       <c r="J112">
-        <v>3.524653043301146</v>
+        <v>3.880678603230554</v>
       </c>
       <c r="K112">
         <v>0</v>
@@ -4976,7 +4976,7 @@
         <v>4885500</v>
       </c>
       <c r="E113">
-        <v>1139</v>
+        <v>1144</v>
       </c>
       <c r="F113">
         <v>21</v>
@@ -4991,10 +4991,10 @@
         <v>4.298434141848326</v>
       </c>
       <c r="J113">
-        <v>233.1388803602497</v>
+        <v>234.1623170606898</v>
       </c>
       <c r="K113">
-        <v>1.843722563652327</v>
+        <v>1.835664335664336</v>
       </c>
     </row>
     <row r="114">
@@ -5017,10 +5017,10 @@
         <v>4829483</v>
       </c>
       <c r="E114">
-        <v>2903</v>
+        <v>3224</v>
       </c>
       <c r="F114">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G114">
         <v>59.54</v>
@@ -5029,13 +5029,13 @@
         <v>3.04</v>
       </c>
       <c r="I114">
-        <v>2.691799515600324</v>
+        <v>3.520045520400424</v>
       </c>
       <c r="J114">
-        <v>601.0995379836723</v>
+        <v>667.5662798688804</v>
       </c>
       <c r="K114">
-        <v>0.4478126076472614</v>
+        <v>0.5272952853598015</v>
       </c>
     </row>
     <row r="115">
@@ -5058,10 +5058,10 @@
         <v>212215030</v>
       </c>
       <c r="E115">
-        <v>24073</v>
+        <v>29465</v>
       </c>
       <c r="F115">
-        <v>564</v>
+        <v>639</v>
       </c>
       <c r="G115">
         <v>56.45</v>
@@ -5070,13 +5070,13 @@
         <v>4.26</v>
       </c>
       <c r="I115">
-        <v>2.657681692008337</v>
+        <v>3.011096810626467</v>
       </c>
       <c r="J115">
-        <v>113.4368286732566</v>
+        <v>138.8450196011093</v>
       </c>
       <c r="K115">
-        <v>2.342873758983093</v>
+        <v>2.168674698795181</v>
       </c>
     </row>
     <row r="116">
@@ -5099,10 +5099,10 @@
         <v>4176873</v>
       </c>
       <c r="E116">
-        <v>7731</v>
+        <v>8282</v>
       </c>
       <c r="F116">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="G116">
         <v>67.88</v>
@@ -5111,13 +5111,13 @@
         <v>7.08</v>
       </c>
       <c r="I116">
-        <v>52.19215427426211</v>
+        <v>56.74101175688129</v>
       </c>
       <c r="J116">
-        <v>1850.90616832257</v>
+        <v>1982.823035318527</v>
       </c>
       <c r="K116">
-        <v>2.819816323890829</v>
+        <v>2.861627626177252</v>
       </c>
     </row>
     <row r="117">
@@ -5140,10 +5140,10 @@
         <v>31989256</v>
       </c>
       <c r="E117">
-        <v>54817</v>
+        <v>65015</v>
       </c>
       <c r="F117">
-        <v>1533</v>
+        <v>1814</v>
       </c>
       <c r="G117">
         <v>69.02</v>
@@ -5152,13 +5152,13 @@
         <v>6.49</v>
       </c>
       <c r="I117">
-        <v>47.92233992563003</v>
+        <v>56.7065392205433</v>
       </c>
       <c r="J117">
-        <v>1713.606593413739</v>
+        <v>2032.401128678954</v>
       </c>
       <c r="K117">
-        <v>2.796577703996935</v>
+        <v>2.790125355687149</v>
       </c>
     </row>
     <row r="118">
@@ -5181,10 +5181,10 @@
         <v>106651922</v>
       </c>
       <c r="E118">
-        <v>10004</v>
+        <v>10610</v>
       </c>
       <c r="F118">
-        <v>658</v>
+        <v>704</v>
       </c>
       <c r="G118">
         <v>58.92</v>
@@ -5193,13 +5193,13 @@
         <v>6.71</v>
       </c>
       <c r="I118">
-        <v>6.169602831911458</v>
+        <v>6.600912452379433</v>
       </c>
       <c r="J118">
-        <v>93.80046615568729</v>
+        <v>99.482501590548</v>
       </c>
       <c r="K118">
-        <v>6.577369052379048</v>
+        <v>6.635249764373233</v>
       </c>
     </row>
     <row r="119">
@@ -5263,10 +5263,10 @@
         <v>37978548</v>
       </c>
       <c r="E120">
-        <v>14740</v>
+        <v>15651</v>
       </c>
       <c r="F120">
-        <v>733</v>
+        <v>785</v>
       </c>
       <c r="G120">
         <v>73.53</v>
@@ -5275,13 +5275,13 @@
         <v>6.67</v>
       </c>
       <c r="I120">
-        <v>19.30036925055692</v>
+        <v>20.66956324923217</v>
       </c>
       <c r="J120">
-        <v>388.1138373167926</v>
+        <v>412.1010629474302</v>
       </c>
       <c r="K120">
-        <v>4.972862957937584</v>
+        <v>5.015653951824165</v>
       </c>
     </row>
     <row r="121">
@@ -5304,10 +5304,10 @@
         <v>10281762</v>
       </c>
       <c r="E121">
-        <v>26182</v>
+        <v>27406</v>
       </c>
       <c r="F121">
-        <v>1089</v>
+        <v>1126</v>
       </c>
       <c r="G121">
         <v>84.23</v>
@@ -5316,13 +5316,13 @@
         <v>7.84</v>
       </c>
       <c r="I121">
-        <v>105.9156981069976</v>
+        <v>109.5143030931858</v>
       </c>
       <c r="J121">
-        <v>2546.450695902122</v>
+        <v>2665.496439228996</v>
       </c>
       <c r="K121">
-        <v>4.159346115651974</v>
+        <v>4.108589359994162</v>
       </c>
     </row>
     <row r="122">
@@ -5345,7 +5345,7 @@
         <v>6956071</v>
       </c>
       <c r="E122">
-        <v>440</v>
+        <v>689</v>
       </c>
       <c r="F122">
         <v>10</v>
@@ -5360,10 +5360,10 @@
         <v>1.437593147050972</v>
       </c>
       <c r="J122">
-        <v>63.25409847024276</v>
+        <v>99.05016783181195</v>
       </c>
       <c r="K122">
-        <v>2.272727272727273</v>
+        <v>1.451378809869376</v>
       </c>
     </row>
     <row r="123">
@@ -5386,10 +5386,10 @@
         <v>2781677</v>
       </c>
       <c r="E123">
-        <v>17972</v>
+        <v>21331</v>
       </c>
       <c r="F123">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G123">
         <v>60.17</v>
@@ -5398,13 +5398,13 @@
         <v>3.19</v>
       </c>
       <c r="I123">
-        <v>4.313944429924826</v>
+        <v>4.673439799085227</v>
       </c>
       <c r="J123">
-        <v>6460.850774550748</v>
+        <v>7668.395719560538</v>
       </c>
       <c r="K123">
-        <v>0.06677053193857112</v>
+        <v>0.06094416576813089</v>
       </c>
     </row>
     <row r="124">
@@ -5427,10 +5427,10 @@
         <v>144478050</v>
       </c>
       <c r="E124">
-        <v>165929</v>
+        <v>198676</v>
       </c>
       <c r="F124">
-        <v>1537</v>
+        <v>1827</v>
       </c>
       <c r="G124">
         <v>50.55</v>
@@ -5439,13 +5439,13 @@
         <v>3.17</v>
       </c>
       <c r="I124">
-        <v>10.63829419070925</v>
+        <v>12.64551950971099</v>
       </c>
       <c r="J124">
-        <v>1148.472034333243</v>
+        <v>1375.129301648243</v>
       </c>
       <c r="K124">
-        <v>0.9262998029277582</v>
+        <v>0.9195876703779017</v>
       </c>
     </row>
     <row r="125">
@@ -5468,7 +5468,7 @@
         <v>12301939</v>
       </c>
       <c r="E125">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="F125">
         <v>0</v>
@@ -5483,7 +5483,7 @@
         <v>0</v>
       </c>
       <c r="J125">
-        <v>21.78518362024068</v>
+        <v>22.76063960323653</v>
       </c>
       <c r="K125">
         <v>0</v>
@@ -5509,10 +5509,10 @@
         <v>33699947</v>
       </c>
       <c r="E126">
-        <v>31938</v>
+        <v>37136</v>
       </c>
       <c r="F126">
-        <v>209</v>
+        <v>239</v>
       </c>
       <c r="G126">
         <v>33.98</v>
@@ -5521,13 +5521,13 @@
         <v>1.93</v>
       </c>
       <c r="I126">
-        <v>6.201790168987507</v>
+        <v>7.091999284153177</v>
       </c>
       <c r="J126">
-        <v>947.716624005373</v>
+        <v>1101.960190026412</v>
       </c>
       <c r="K126">
-        <v>0.6543928862170455</v>
+        <v>0.6435803532959931</v>
       </c>
     </row>
     <row r="127">
@@ -5550,10 +5550,10 @@
         <v>41801533</v>
       </c>
       <c r="E127">
-        <v>852</v>
+        <v>1164</v>
       </c>
       <c r="F127">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G127">
         <v>26.44</v>
@@ -5562,13 +5562,13 @@
         <v>2.15</v>
       </c>
       <c r="I127">
-        <v>1.172205813600186</v>
+        <v>1.531044327967589</v>
       </c>
       <c r="J127">
-        <v>20.38202761606853</v>
+        <v>27.84586871491053</v>
       </c>
       <c r="K127">
-        <v>5.751173708920188</v>
+        <v>5.498281786941581</v>
       </c>
     </row>
     <row r="128">
@@ -5591,10 +5591,10 @@
         <v>15854360</v>
       </c>
       <c r="E128">
-        <v>1433</v>
+        <v>1634</v>
       </c>
       <c r="F128">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G128">
         <v>73.28</v>
@@ -5603,13 +5603,13 @@
         <v>6.15</v>
       </c>
       <c r="I128">
-        <v>0.7568895874699452</v>
+        <v>1.072260248915756</v>
       </c>
       <c r="J128">
-        <v>90.38523157036929</v>
+        <v>103.0631321604909</v>
       </c>
       <c r="K128">
-        <v>0.8374040474528961</v>
+        <v>1.040391676866585</v>
       </c>
     </row>
     <row r="129">
@@ -5632,7 +5632,7 @@
         <v>5638676</v>
       </c>
       <c r="E129">
-        <v>20198</v>
+        <v>22460</v>
       </c>
       <c r="F129">
         <v>20</v>
@@ -5647,10 +5647,10 @@
         <v>3.546931939341789</v>
       </c>
       <c r="J129">
-        <v>3582.046565541272</v>
+        <v>3983.204567880829</v>
       </c>
       <c r="K129">
-        <v>0.09901970492127933</v>
+        <v>0.08904719501335707</v>
       </c>
     </row>
     <row r="130">
@@ -5673,10 +5673,10 @@
         <v>7650154</v>
       </c>
       <c r="E130">
-        <v>225</v>
+        <v>291</v>
       </c>
       <c r="F130">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G130">
         <v>69.27</v>
@@ -5685,13 +5685,13 @@
         <v>4.66</v>
       </c>
       <c r="I130">
-        <v>1.830028519687316</v>
+        <v>2.352893811026549</v>
       </c>
       <c r="J130">
-        <v>29.41117263783187</v>
+        <v>38.03844994492921</v>
       </c>
       <c r="K130">
-        <v>6.222222222222222</v>
+        <v>6.185567010309279</v>
       </c>
     </row>
     <row r="131">
@@ -5714,10 +5714,10 @@
         <v>6420744</v>
       </c>
       <c r="E131">
-        <v>695</v>
+        <v>889</v>
       </c>
       <c r="F131">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G131">
         <v>72.76000000000001</v>
@@ -5726,13 +5726,13 @@
         <v>6.43</v>
       </c>
       <c r="I131">
-        <v>2.336177863499931</v>
+        <v>2.647668245299922</v>
       </c>
       <c r="J131">
-        <v>108.2429076754968</v>
+        <v>138.4574747100959</v>
       </c>
       <c r="K131">
-        <v>2.158273381294964</v>
+        <v>1.912260967379078</v>
       </c>
     </row>
     <row r="132">
@@ -5796,10 +5796,10 @@
         <v>5447011</v>
       </c>
       <c r="E133">
-        <v>1429</v>
+        <v>1455</v>
       </c>
       <c r="F133">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G133">
         <v>84.48999999999999</v>
@@ -5808,13 +5808,13 @@
         <v>7.16</v>
       </c>
       <c r="I133">
-        <v>4.589673125315884</v>
+        <v>4.77326005032852</v>
       </c>
       <c r="J133">
-        <v>262.3457158430559</v>
+        <v>267.1189758933845</v>
       </c>
       <c r="K133">
-        <v>1.749475157452764</v>
+        <v>1.786941580756014</v>
       </c>
     </row>
     <row r="134">
@@ -5837,10 +5837,10 @@
         <v>2067372</v>
       </c>
       <c r="E134">
-        <v>1448</v>
+        <v>1454</v>
       </c>
       <c r="F134">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G134">
         <v>78.3</v>
@@ -5849,13 +5849,13 @@
         <v>7.5</v>
       </c>
       <c r="I134">
-        <v>47.8868824768837</v>
+        <v>48.85429424409347</v>
       </c>
       <c r="J134">
-        <v>700.4061194598747</v>
+        <v>703.308354761504</v>
       </c>
       <c r="K134">
-        <v>6.837016574585636</v>
+        <v>6.946354883081156</v>
       </c>
     </row>
     <row r="135">
@@ -5878,10 +5878,10 @@
         <v>10183175</v>
       </c>
       <c r="E135">
-        <v>23918</v>
+        <v>25921</v>
       </c>
       <c r="F135">
-        <v>2941</v>
+        <v>3220</v>
       </c>
       <c r="G135">
         <v>91.73</v>
@@ -5890,13 +5890,13 @@
         <v>9.390000000000001</v>
       </c>
       <c r="I135">
-        <v>288.8097278108252</v>
+        <v>316.2078624790402</v>
       </c>
       <c r="J135">
-        <v>2348.776290302386</v>
+        <v>2545.473292956273</v>
       </c>
       <c r="K135">
-        <v>12.29617861025169</v>
+        <v>12.42236024844721</v>
       </c>
     </row>
     <row r="136">
@@ -5919,7 +5919,7 @@
         <v>1367000</v>
       </c>
       <c r="E136">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="F136">
         <v>2</v>
@@ -5934,10 +5934,10 @@
         <v>1.463057790782736</v>
       </c>
       <c r="J136">
-        <v>89.97805413313826</v>
+        <v>119.239209948793</v>
       </c>
       <c r="K136">
-        <v>1.626016260162602</v>
+        <v>1.226993865030675</v>
       </c>
     </row>
     <row r="137">
@@ -5960,7 +5960,7 @@
         <v>16906283</v>
       </c>
       <c r="E137">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F137">
         <v>3</v>
@@ -5975,10 +5975,10 @@
         <v>0.1774488218374198</v>
       </c>
       <c r="J137">
-        <v>2.661732327561298</v>
+        <v>2.780031542119578</v>
       </c>
       <c r="K137">
-        <v>6.666666666666667</v>
+        <v>6.382978723404255</v>
       </c>
     </row>
     <row r="138">
@@ -6001,10 +6001,10 @@
         <v>15477751</v>
       </c>
       <c r="E138">
-        <v>170</v>
+        <v>322</v>
       </c>
       <c r="F138">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="G138">
         <v>60.34</v>
@@ -6013,13 +6013,13 @@
         <v>1.5</v>
       </c>
       <c r="I138">
-        <v>1.098350787527206</v>
+        <v>2.002874965490788</v>
       </c>
       <c r="J138">
-        <v>10.98350787527206</v>
+        <v>20.80405609316237</v>
       </c>
       <c r="K138">
-        <v>10</v>
+        <v>9.627329192546584</v>
       </c>
     </row>
     <row r="139">
@@ -6042,10 +6042,10 @@
         <v>7889094</v>
       </c>
       <c r="E139">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="F139">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G139">
         <v>69.25</v>
@@ -6054,13 +6054,13 @@
         <v>3.05</v>
       </c>
       <c r="I139">
-        <v>1.140815409221895</v>
+        <v>1.267572676913217</v>
       </c>
       <c r="J139">
-        <v>16.22493026448918</v>
+        <v>19.39386195677222</v>
       </c>
       <c r="K139">
-        <v>7.03125</v>
+        <v>6.535947712418301</v>
       </c>
     </row>
     <row r="140">
@@ -6083,10 +6083,10 @@
         <v>69428524</v>
       </c>
       <c r="E140">
-        <v>2989</v>
+        <v>3004</v>
       </c>
       <c r="F140">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G140">
         <v>55.31</v>
@@ -6095,13 +6095,13 @@
         <v>4.63</v>
       </c>
       <c r="I140">
-        <v>0.7921816111199483</v>
+        <v>0.8065849131403111</v>
       </c>
       <c r="J140">
-        <v>43.05146973886411</v>
+        <v>43.26751926916955</v>
       </c>
       <c r="K140">
-        <v>1.840080294412847</v>
+        <v>1.864181091877497</v>
       </c>
     </row>
     <row r="141">
@@ -6124,10 +6124,10 @@
         <v>9100837</v>
       </c>
       <c r="E141">
-        <v>379</v>
+        <v>612</v>
       </c>
       <c r="F141">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G141">
         <v>49.73</v>
@@ -6136,13 +6136,13 @@
         <v>1.93</v>
       </c>
       <c r="I141">
-        <v>0.8790400267579784</v>
+        <v>2.197600066894946</v>
       </c>
       <c r="J141">
-        <v>41.64452126765923</v>
+        <v>67.24656204698536</v>
       </c>
       <c r="K141">
-        <v>2.110817941952507</v>
+        <v>3.267973856209151</v>
       </c>
     </row>
     <row r="142">
@@ -6206,10 +6206,10 @@
         <v>11565204</v>
       </c>
       <c r="E143">
-        <v>1025</v>
+        <v>1032</v>
       </c>
       <c r="F143">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G143">
         <v>67.78</v>
@@ -6218,13 +6218,13 @@
         <v>6.32</v>
       </c>
       <c r="I143">
-        <v>3.718049417891808</v>
+        <v>3.890981948956542</v>
       </c>
       <c r="J143">
-        <v>88.6279221706768</v>
+        <v>89.23318602940337</v>
       </c>
       <c r="K143">
-        <v>4.195121951219512</v>
+        <v>4.36046511627907</v>
       </c>
     </row>
     <row r="144">
@@ -6247,10 +6247,10 @@
         <v>82319724</v>
       </c>
       <c r="E144">
-        <v>131744</v>
+        <v>137115</v>
       </c>
       <c r="F144">
-        <v>3584</v>
+        <v>3739</v>
       </c>
       <c r="G144">
         <v>47.02</v>
@@ -6259,13 +6259,13 @@
         <v>4.88</v>
       </c>
       <c r="I144">
-        <v>43.53756093740061</v>
+        <v>45.42046326588753</v>
       </c>
       <c r="J144">
-        <v>1600.394092672128</v>
+        <v>1665.639695293439</v>
       </c>
       <c r="K144">
-        <v>2.720427495749332</v>
+        <v>2.726908069868359</v>
       </c>
     </row>
     <row r="145">
@@ -6288,10 +6288,10 @@
         <v>56318348</v>
       </c>
       <c r="E145">
-        <v>480</v>
+        <v>509</v>
       </c>
       <c r="F145">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G145">
         <v>69.34999999999999</v>
@@ -6300,13 +6300,13 @@
         <v>5.47</v>
       </c>
       <c r="I145">
-        <v>0.3196116476996094</v>
+        <v>0.3728802556495442</v>
       </c>
       <c r="J145">
-        <v>8.522977271989582</v>
+        <v>9.037907148838954</v>
       </c>
       <c r="K145">
-        <v>3.75</v>
+        <v>4.12573673870334</v>
       </c>
     </row>
     <row r="146">
@@ -6329,7 +6329,7 @@
         <v>42723139</v>
       </c>
       <c r="E146">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="F146">
         <v>0</v>
@@ -6344,7 +6344,7 @@
         <v>0</v>
       </c>
       <c r="J146">
-        <v>2.293838942873556</v>
+        <v>2.715156299727883</v>
       </c>
       <c r="K146">
         <v>0</v>
@@ -6370,10 +6370,10 @@
         <v>44622516</v>
       </c>
       <c r="E147">
-        <v>13184</v>
+        <v>14710</v>
       </c>
       <c r="F147">
-        <v>327</v>
+        <v>376</v>
       </c>
       <c r="G147">
         <v>66.81</v>
@@ -6382,13 +6382,13 @@
         <v>5.69</v>
       </c>
       <c r="I147">
-        <v>7.328139004981252</v>
+        <v>8.426239345177219</v>
       </c>
       <c r="J147">
-        <v>295.4562221457884</v>
+        <v>329.6542041690343</v>
       </c>
       <c r="K147">
-        <v>2.480279126213592</v>
+        <v>2.556084296397009</v>
       </c>
     </row>
     <row r="148">
@@ -6411,10 +6411,10 @@
         <v>3449299</v>
       </c>
       <c r="E148">
-        <v>775</v>
+        <v>702</v>
       </c>
       <c r="F148">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G148">
         <v>82.56999999999999</v>
@@ -6423,13 +6423,13 @@
         <v>8.119999999999999</v>
       </c>
       <c r="I148">
-        <v>4.928537653592802</v>
+        <v>5.218451633215908</v>
       </c>
       <c r="J148">
-        <v>224.6833342079072</v>
+        <v>203.5196136954204</v>
       </c>
       <c r="K148">
-        <v>2.193548387096774</v>
+        <v>2.564102564102564</v>
       </c>
     </row>
     <row r="149">
@@ -6452,10 +6452,10 @@
         <v>327167434</v>
       </c>
       <c r="E149">
-        <v>1228603</v>
+        <v>1309541</v>
       </c>
       <c r="F149">
-        <v>73431</v>
+        <v>78794</v>
       </c>
       <c r="G149">
         <v>76.12</v>
@@ -6464,13 +6464,13 @@
         <v>7.98</v>
       </c>
       <c r="I149">
-        <v>224.4447104720087</v>
+        <v>240.8369287757412</v>
       </c>
       <c r="J149">
-        <v>3755.272904087391</v>
+        <v>4002.663052337905</v>
       </c>
       <c r="K149">
-        <v>5.976788270906062</v>
+        <v>6.016917377920966</v>
       </c>
     </row>
     <row r="150">
@@ -6493,7 +6493,7 @@
         <v>32955400</v>
       </c>
       <c r="E150">
-        <v>2233</v>
+        <v>2387</v>
       </c>
       <c r="F150">
         <v>10</v>
@@ -6508,10 +6508,10 @@
         <v>0.3034404073384028</v>
       </c>
       <c r="J150">
-        <v>67.75824295866535</v>
+        <v>72.43122523167675</v>
       </c>
       <c r="K150">
-        <v>0.4478280340349305</v>
+        <v>0.4189359028068705</v>
       </c>
     </row>
     <row r="151">
@@ -6534,7 +6534,7 @@
         <v>28870195</v>
       </c>
       <c r="E151">
-        <v>379</v>
+        <v>402</v>
       </c>
       <c r="F151">
         <v>10</v>
@@ -6549,10 +6549,10 @@
         <v>0.3463779860163743</v>
       </c>
       <c r="J151">
-        <v>13.12772567002059</v>
+        <v>13.92439503785825</v>
       </c>
       <c r="K151">
-        <v>2.638522427440633</v>
+        <v>2.487562189054727</v>
       </c>
     </row>
     <row r="152">
@@ -6575,7 +6575,7 @@
         <v>95540395</v>
       </c>
       <c r="E152">
-        <v>271</v>
+        <v>288</v>
       </c>
       <c r="F152">
         <v>0</v>
@@ -6590,7 +6590,7 @@
         <v>0</v>
       </c>
       <c r="J152">
-        <v>2.836496541593742</v>
+        <v>3.014431748999991</v>
       </c>
       <c r="K152">
         <v>0</v>
@@ -6616,10 +6616,10 @@
         <v>28498687</v>
       </c>
       <c r="E153">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F153">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G153">
         <v>34.2</v>
@@ -6628,13 +6628,13 @@
         <v>2.07</v>
       </c>
       <c r="I153">
-        <v>0.1754466793505259</v>
+        <v>0.2456253510907362</v>
       </c>
       <c r="J153">
-        <v>0.8772333967526293</v>
+        <v>1.193037419583576</v>
       </c>
       <c r="K153">
-        <v>20</v>
+        <v>20.58823529411764</v>
       </c>
     </row>
     <row r="154">
@@ -6657,10 +6657,10 @@
         <v>57779622</v>
       </c>
       <c r="E154">
-        <v>7808</v>
+        <v>9420</v>
       </c>
       <c r="F154">
-        <v>153</v>
+        <v>186</v>
       </c>
       <c r="G154">
         <v>79.88</v>
@@ -6669,13 +6669,13 @@
         <v>7.24</v>
       </c>
       <c r="I154">
-        <v>2.647992401196394</v>
+        <v>3.219128017140714</v>
       </c>
       <c r="J154">
-        <v>135.1341481604016</v>
+        <v>163.0332576422878</v>
       </c>
       <c r="K154">
-        <v>1.95952868852459</v>
+        <v>1.974522292993631</v>
       </c>
     </row>
     <row r="155">
@@ -6698,10 +6698,10 @@
         <v>17351822</v>
       </c>
       <c r="E155">
-        <v>146</v>
+        <v>252</v>
       </c>
       <c r="F155">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G155">
         <v>63.52</v>
@@ -6710,13 +6710,13 @@
         <v>5.68</v>
       </c>
       <c r="I155">
-        <v>0.2305233421596879</v>
+        <v>0.4034158487794538</v>
       </c>
       <c r="J155">
-        <v>8.414101988828607</v>
+        <v>14.52297055606034</v>
       </c>
       <c r="K155">
-        <v>2.73972602739726</v>
+        <v>2.777777777777778</v>
       </c>
     </row>
     <row r="156">
@@ -6739,7 +6739,7 @@
         <v>14439018</v>
       </c>
       <c r="E156">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F156">
         <v>4</v>
@@ -6754,10 +6754,10 @@
         <v>0.2770271496302588</v>
       </c>
       <c r="J156">
-        <v>2.3547307718572</v>
+        <v>2.493244346672329</v>
       </c>
       <c r="K156">
-        <v>11.76470588235294</v>
+        <v>11.11111111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>